<commit_message>
atualização no codigo para maior desempenho
</commit_message>
<xml_diff>
--- a/Contatos.xlsx
+++ b/Contatos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29324"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02A3AB11-4300-4F23-914F-B7E0B6E96BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E79933AF-D98D-4024-ACD3-0BD3BE881D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Nome</t>
   </si>
@@ -43,312 +43,95 @@
   </si>
   <si>
     <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 43</t>
+Já disponível na loja ⚠️
+Oakley Stractus Premium
+38 ao 43
+R$ 279,90 em ate 10x sem juros no cartão
+https://chat.whatsapp.com/K2ceC07pH7h2lMCYcRUJfB?mode=ems_copy_t</t>
   </si>
   <si>
     <t>MeN Moda Masc grupo</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 44</t>
-  </si>
-  <si>
     <t>TROCA TROCA</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 45</t>
-  </si>
-  <si>
     <t>MULT PREÇOS (Vendas e Notícias)</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 46</t>
-  </si>
-  <si>
     <t>💰💰FEIRA LIVRE MG💰💰</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 47</t>
-  </si>
-  <si>
     <t>OLX Poços de Caldas e região</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 48</t>
-  </si>
-  <si>
     <t>VENDAS ZONA LESTE</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 49</t>
-  </si>
-  <si>
     <t>Classificados ZONA SUL ‼️‼️</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 50</t>
-  </si>
-  <si>
     <t>Vendas Poços de Caldas</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 51</t>
-  </si>
-  <si>
     <t>Compra e venda Poços C 🐰</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 52</t>
-  </si>
-  <si>
     <t>Troca&amp;VendePoçosdeCaldas3</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 53</t>
-  </si>
-  <si>
     <t>💸Classificados Poços 1⃣</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 54</t>
-  </si>
-  <si>
     <t>CLASSIFICADOS POÇOS. (2)</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 55</t>
-  </si>
-  <si>
     <t>🇧🇷Aqui Vende Mais1️⃣Poços🇧🇷</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 56</t>
-  </si>
-  <si>
     <t>COMÉRCIO LOCAL SUL MG</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 57</t>
-  </si>
-  <si>
     <t>ANUNCIE + E VENDA +</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 58</t>
-  </si>
-  <si>
     <t>STA TERESA / SÃO BENTO</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 59</t>
-  </si>
-  <si>
     <t>Vende - se &amp; Trocas</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 60</t>
-  </si>
-  <si>
     <t>📣 Anuncia Zona Sul 📣</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 61</t>
-  </si>
-  <si>
     <t>TUDO A VENDA 😁</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 62</t>
-  </si>
-  <si>
     <t>Compra e Venda PUC</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 63</t>
-  </si>
-  <si>
     <t>Desapega aí!</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 64</t>
-  </si>
-  <si>
     <t>😊VENDA DE TUDO😊    (Poços de Caldas)</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 65</t>
-  </si>
-  <si>
     <t>Bons negócios - Poços 🤝🏽</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 66</t>
-  </si>
-  <si>
     <t>BOM DE NEGÓCIOS POÇOS</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 67</t>
-  </si>
-  <si>
     <t>Vendas Trocas de Tudo</t>
   </si>
   <si>
-    <t>PRONTA ENTREGA
-Já disponível na loja⚠️
-Vans ultrarange neo prime 
-Couro 
-Bege 
-R$ 219,90 em ate 10x sem juros no cartão
-Disponível 34 ao 68</t>
+    <t>Bairro: Jd ipê, Caio Junqueira,Nova Aurora,Jd São Paulo,Monte verde. Azaléia, hortência,amarílis.</t>
+  </si>
+  <si>
+    <t>Conexão Empreendedora 🤝💡💰🛍️💼</t>
+  </si>
+  <si>
+    <t>Grupão São José Rio Pardo</t>
   </si>
 </sst>
 </file>
@@ -737,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -757,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="102.75">
+    <row r="2" spans="1:2" ht="175.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -765,204 +548,236 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="102.75">
+    <row r="3" spans="1:2" ht="175.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="175.5">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="102.75">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="175.5">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="175.5">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="102.75">
-      <c r="A5" t="s">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="175.5">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="175.5">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="102.75">
-      <c r="A6" t="s">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="175.5">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="175.5">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="102.75">
-      <c r="A7" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="175.5">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="175.5">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="102.75">
-      <c r="A8" t="s">
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="175.5">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="175.5">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="102.75">
-      <c r="A9" t="s">
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="175.5">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="175.5">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="102.75">
-      <c r="A10" t="s">
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="175.5">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="175.5">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="102.75">
-      <c r="A11" t="s">
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="175.5">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="175.5">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="102.75">
-      <c r="A12" t="s">
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="175.5">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="175.5">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="102.75">
-      <c r="A13" t="s">
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="175.5">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="175.5">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="102.75">
-      <c r="A14" t="s">
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="175.5">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="175.5">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="102.75">
-      <c r="A15" t="s">
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="175.5">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="175.5">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="102.75">
-      <c r="A16" t="s">
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="175.5">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="175.5">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="175.5">
+      <c r="A31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="102.75">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="102.75">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="102.75">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="102.75">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="102.75">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="102.75">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="102.75">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="102.75">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="102.75">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="102.75">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="102.75">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>